<commit_message>
.sphr diagram; menu rearangement; images
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Environmental.xlsx
+++ b/output/StructureDefinition-Environmental.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.3.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-10T00:26:50-05:00</t>
+    <t>2022-05-10T00:36:03-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
conformance table; conceptmaps; sliced bundle profile; record keeping guidance; JohnDoe examples removed
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Environmental.xlsx
+++ b/output/StructureDefinition-Environmental.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.9</t>
+    <t>0.3.10</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-21T12:25:18-04:00</t>
+    <t>2022-09-28T23:23:22-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>